<commit_message>
Fixed bug with queues
Former-commit-id: aec5836ba1367044f5cf0c83667e9c8c99469543
</commit_message>
<xml_diff>
--- a/data/adapter_sdm/flexis/Szenario1-84Sek_gut_neu.xlsx
+++ b/data/adapter_sdm/flexis/Szenario1-84Sek_gut_neu.xlsx
@@ -12882,22 +12882,22 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>f1b5014b-9d85-11ed-96f4-86d241e2ee3e</t>
+          <t>e075e7af-9d86-11ed-a741-86d241e2ee3e</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>f1b5014b-9d85-11ed-96f4-86d241e2ee3e</t>
+          <t>e075e7af-9d86-11ed-a741-86d241e2ee3e</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>SchneckenradMontage</t>
+          <t>SensordeckelMontage</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>SchneckenradMontage</t>
+          <t>SensordeckelMontage</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -12907,17 +12907,17 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>~SchneckenradMontage~</t>
+          <t>~SensordeckelMontage~</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Setup_SchneckenradMontage</t>
+          <t>Setup_SensordeckelMontage</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Duration_SchneckenradMontage</t>
+          <t>Duration_SensordeckelMontage</t>
         </is>
       </c>
       <c r="I6" t="inlineStr"/>

</xml_diff>

<commit_message>
Got running with positions
Former-commit-id: 2ab68d42ff6d53661cc67946c3ace600a0f9851a
</commit_message>
<xml_diff>
--- a/data/adapter_sdm/flexis/Szenario1-84Sek_gut_neu.xlsx
+++ b/data/adapter_sdm/flexis/Szenario1-84Sek_gut_neu.xlsx
@@ -12588,7 +12588,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12662,6 +12662,11 @@
           <t>movementMode:String</t>
         </is>
       </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>location:Point</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -12717,6 +12722,11 @@
           <t>RANDOM</t>
         </is>
       </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>(7.44, 4.96)</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -12772,6 +12782,11 @@
           <t>RANDOM</t>
         </is>
       </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>(2.48, 2.48)</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -12827,6 +12842,11 @@
           <t>RANDOM</t>
         </is>
       </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>(14.88, 9.92)</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -12878,16 +12898,21 @@
           <t>RANDOM</t>
         </is>
       </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>(4.96, 12.4)</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>e075e7af-9d86-11ed-a741-86d241e2ee3e</t>
+          <t>b3e0d6a3-9da9-11ed-b283-86d241e2ee3e</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>e075e7af-9d86-11ed-a741-86d241e2ee3e</t>
+          <t>b3e0d6a3-9da9-11ed-b283-86d241e2ee3e</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -12931,6 +12956,11 @@
       <c r="M6" t="inlineStr">
         <is>
           <t>RANDOM</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>(7.44, 0)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed bug in optimization util and refactored
Former-commit-id: 6ce7cf29d691c824ea3e4b1985917f2321099d2b
</commit_message>
<xml_diff>
--- a/data/adapter_sdm/flexis/Szenario1-84Sek_gut_neu.xlsx
+++ b/data/adapter_sdm/flexis/Szenario1-84Sek_gut_neu.xlsx
@@ -12724,7 +12724,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>(7.44, 4.96)</t>
+          <t>(2.48, 2.48)</t>
         </is>
       </c>
     </row>
@@ -12784,7 +12784,7 @@
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>(2.48, 2.48)</t>
+          <t>(12.4, 14.88)</t>
         </is>
       </c>
     </row>
@@ -12844,7 +12844,7 @@
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>(14.88, 9.92)</t>
+          <t>(14.88, 4.96)</t>
         </is>
       </c>
     </row>
@@ -12900,29 +12900,29 @@
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>(4.96, 12.4)</t>
+          <t>(4.96, 2.48)</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>b3e0d6a3-9da9-11ed-b283-86d241e2ee3e</t>
+          <t>b840c1ec-a003-11ed-8985-86d241e2ee3e</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>b3e0d6a3-9da9-11ed-b283-86d241e2ee3e</t>
+          <t>b840c1ec-a003-11ed-8985-86d241e2ee3e</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>SensordeckelMontage</t>
+          <t>Schmierung</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>SensordeckelMontage</t>
+          <t>Schmierung</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -12932,17 +12932,13 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>~SensordeckelMontage~</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Setup_SensordeckelMontage</t>
-        </is>
-      </c>
+          <t>~Schmierung~</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Duration_SensordeckelMontage</t>
+          <t>Duration_Schmierung</t>
         </is>
       </c>
       <c r="I6" t="inlineStr"/>
@@ -12960,7 +12956,7 @@
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>(7.44, 0)</t>
+          <t>(12.4, 2.48)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed blocking problem and removed deadlock router
Former-commit-id: 0df9ef7fc9a2770c636b2419788856670aca8b0b
</commit_message>
<xml_diff>
--- a/data/adapter_sdm/flexis/Szenario1-84Sek_gut_neu.xlsx
+++ b/data/adapter_sdm/flexis/Szenario1-84Sek_gut_neu.xlsx
@@ -12724,7 +12724,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>(2.48, 2.48)</t>
+          <t>(4.96, 2.48)</t>
         </is>
       </c>
     </row>
@@ -12784,7 +12784,7 @@
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>(12.4, 14.88)</t>
+          <t>(12.4, 7.44)</t>
         </is>
       </c>
     </row>
@@ -12844,7 +12844,7 @@
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>(14.88, 4.96)</t>
+          <t>(2.48, 7.44)</t>
         </is>
       </c>
     </row>
@@ -12900,19 +12900,19 @@
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>(4.96, 2.48)</t>
+          <t>(9.92, 14.88)</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>b840c1ec-a003-11ed-8985-86d241e2ee3e</t>
+          <t>35d81952-aaec-11ed-9ab6-00155d20abc6</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>b840c1ec-a003-11ed-8985-86d241e2ee3e</t>
+          <t>35d81952-aaec-11ed-9ab6-00155d20abc6</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -12956,7 +12956,7 @@
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>(12.4, 2.48)</t>
+          <t>(9.92, 7.44)</t>
         </is>
       </c>
     </row>

</xml_diff>